<commit_message>
run rev with log
</commit_message>
<xml_diff>
--- a/re_cap/Installed_RE_Capacity_China.xlsx
+++ b/re_cap/Installed_RE_Capacity_China.xlsx
@@ -1,21 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcb\Dropbox (MIT)\FofS\India\genx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcb\Documents\Github\rev-india\re_cap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{5874F80C-D948-49FC-BA18-1363B7D9F9D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{800518B2-2DED-4767-901F-44302E26F2C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="-110" windowWidth="24890" windowHeight="14620"/>
+    <workbookView xWindow="3900" yWindow="1470" windowWidth="18500" windowHeight="10510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Installed_RE_Capacity_China" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -40,7 +50,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -874,11 +884,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1138,18 +1148,18 @@
         <v>2030</v>
       </c>
       <c r="B22">
-        <v>897</v>
+        <v>980</v>
       </c>
       <c r="C22">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D22">
-        <f t="shared" ref="D22:E23" si="0">(B22/B21)^(1/(A22-A21))-1</f>
-        <v>9.8805648315637429E-2</v>
+        <f t="shared" ref="D22:D23" si="0">(B22/B21)^(1/(A22-A21))-1</f>
+        <v>0.11842691472014466</v>
       </c>
       <c r="E22">
         <f t="shared" ref="E22:E23" si="1">(C22/C21)^(1/(A22-A21))-1</f>
-        <v>7.9009688167268166E-2</v>
+        <v>7.819101523029115E-2</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -1157,18 +1167,18 @@
         <v>2040</v>
       </c>
       <c r="B23">
-        <v>1506</v>
+        <v>1826</v>
       </c>
       <c r="C23">
-        <v>875</v>
+        <v>904</v>
       </c>
       <c r="D23">
         <f t="shared" si="0"/>
-        <v>5.318157546991964E-2</v>
+        <v>6.4210328929386051E-2</v>
       </c>
       <c r="E23">
         <f t="shared" si="1"/>
-        <v>5.1810284647477722E-2</v>
+        <v>5.5645908111642939E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>